<commit_message>
small fixes to the MMV files
</commit_message>
<xml_diff>
--- a/data/mmv-implementation.xlsx
+++ b/data/mmv-implementation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamilami\all\buildings\BuildME MMV\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamilami\all\buildings\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55D2148-4B33-461E-9605-AC9D61133957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72A3E5D-2BA1-437F-85F1-E7AF8C776CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="change" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="147">
   <si>
     <t>People</t>
   </si>
@@ -86,12 +86,6 @@
     <t>OpeningHeight</t>
   </si>
   <si>
-    <t>Building_Type</t>
-  </si>
-  <si>
-    <t>HighRise</t>
-  </si>
-  <si>
     <t>Wind_Pressure_Coefficient_Type</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
   </si>
   <si>
     <t>AirflowNetwork:MultiZone:Component:DetailedOpening</t>
-  </si>
-  <si>
-    <t>Extra_Crack_Length_or_Height_of_Pivoting_Axis</t>
   </si>
   <si>
     <t>Number_of_Sets_of_Opening_Factor_Data</t>
@@ -573,8 +564,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FCC55F2-F857-4667-892F-4B3710709F9F}" name="Table2" displayName="Table2" ref="A1:D69" totalsRowShown="0">
-  <autoFilter ref="A1:D69" xr:uid="{E95F4E3E-AEC5-439A-A7A0-FD25B51BF8E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FCC55F2-F857-4667-892F-4B3710709F9F}" name="Table2" displayName="Table2" ref="A1:D67" totalsRowShown="0">
+  <autoFilter ref="A1:D67" xr:uid="{E95F4E3E-AEC5-439A-A7A0-FD25B51BF8E6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8865D9DB-D431-4975-9229-8C6286E87421}" name="object number"/>
     <tableColumn id="2" xr3:uid="{3D54CA2E-DEDC-44BD-903C-115EE860BDB9}" name="idfobject"/>
@@ -882,15 +873,15 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -904,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -915,10 +906,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -926,13 +917,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -940,13 +931,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -954,13 +945,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -971,7 +962,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -985,23 +976,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD63555F-4595-4051-A932-C63C4CE243F7}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="38.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1013,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1027,7 +1018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1041,7 +1032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1055,7 +1046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1069,900 +1060,872 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>3</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" t="s">
         <v>10</v>
       </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>11</v>
       </c>
       <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
         <v>49</v>
       </c>
-      <c r="C35" t="s">
-        <v>50</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>12</v>
       </c>
       <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
         <v>49</v>
       </c>
-      <c r="C39" t="s">
-        <v>50</v>
-      </c>
       <c r="D39" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>13</v>
       </c>
       <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
         <v>49</v>
       </c>
-      <c r="C43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D43" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>13</v>
-      </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>14</v>
       </c>
       <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
         <v>56</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>14</v>
-      </c>
-      <c r="B48" t="s">
-        <v>55</v>
-      </c>
       <c r="C48" t="s">
-        <v>58</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>15</v>
-      </c>
-      <c r="B50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D50" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>17</v>
       </c>
       <c r="B53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" t="s">
         <v>80</v>
-      </c>
-      <c r="C53" t="s">
-        <v>81</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D54" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D56" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D58" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D59" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D61" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D62" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s">
-        <v>90</v>
-      </c>
-      <c r="D63" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>93</v>
-      </c>
-      <c r="D64" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
         <v>75</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C67" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>18</v>
-      </c>
-      <c r="B68" t="s">
-        <v>74</v>
-      </c>
-      <c r="C68" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>18</v>
-      </c>
-      <c r="B69" t="s">
-        <v>74</v>
-      </c>
-      <c r="C69" t="s">
-        <v>24</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1979,31 +1942,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964C1CC5-826A-4834-B9B7-84A48F0779AC}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" customWidth="1"/>
-    <col min="3" max="3" width="28.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
         <v>134</v>
-      </c>
-      <c r="C1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" t="s">
-        <v>137</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2012,2031 +1975,2031 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F2">
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F3">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="G3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F4">
         <v>1E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F6">
         <v>1.4E-3</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F7">
         <v>1.5999999999999999E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F8">
         <v>1.8E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F9">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F10">
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="G10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F11">
         <v>9.6999999999999994E-4</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F12">
         <v>1.8E-3</v>
       </c>
       <c r="G12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F13">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>125</v>
-      </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F14">
         <v>0.02</v>
       </c>
       <c r="G14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>125</v>
-      </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F15">
         <v>0.02</v>
       </c>
       <c r="G15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>125</v>
-      </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F16">
         <v>0.02</v>
       </c>
       <c r="G16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>125</v>
-      </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F17">
         <v>0.02</v>
       </c>
       <c r="G17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F18">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F19">
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="G19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F20">
         <v>0.01</v>
       </c>
       <c r="G20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F21">
         <v>0.04</v>
       </c>
       <c r="G21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F22">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="G22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F23">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F24">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F25">
         <v>0.02</v>
       </c>
       <c r="G25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F26">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F27">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F28">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F29">
         <v>1.9E-2</v>
       </c>
       <c r="G29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F30">
         <v>1E-4</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F31">
         <v>1.5000000000000001E-4</v>
       </c>
       <c r="G31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F32">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F33">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="G33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E34" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F34">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="G34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F35">
         <v>1.4499999999999999E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F36">
         <v>2E-3</v>
       </c>
       <c r="G36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F37">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>132</v>
-      </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E38" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F38">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="G38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>132</v>
-      </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F39">
         <v>8.5000000000000006E-4</v>
       </c>
       <c r="G39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>132</v>
-      </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F40">
         <v>1E-3</v>
       </c>
       <c r="G40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>132</v>
-      </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F41">
         <v>2E-3</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E42" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F42">
         <v>1E-4</v>
       </c>
       <c r="G42" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F43">
         <v>1.25E-4</v>
       </c>
       <c r="G43" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F44">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="G44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E45" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F45">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F46">
         <v>0.65</v>
       </c>
       <c r="G46" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E47" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F47">
         <v>0.625</v>
       </c>
       <c r="G47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D48" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E48" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F48">
         <v>0.6</v>
       </c>
       <c r="G48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C49" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E49" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F49">
         <v>0.6</v>
       </c>
       <c r="G49" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F50">
         <v>0.65</v>
       </c>
       <c r="G50" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E51" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F51">
         <v>0.625</v>
       </c>
       <c r="G51" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D52" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E52" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F52">
         <v>0.6</v>
       </c>
       <c r="G52" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C53" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D53" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E53" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F53">
         <v>0.6</v>
       </c>
       <c r="G53" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E54" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F54">
         <v>0.65</v>
       </c>
       <c r="G54" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D55" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E55" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F55">
         <v>0.65500000000000003</v>
       </c>
       <c r="G55" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C56" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D56" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E56" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F56">
         <v>0.66</v>
       </c>
       <c r="G56" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D57" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E57" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F57">
         <v>0.66</v>
       </c>
       <c r="G57" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E58" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F58">
         <v>0.6</v>
       </c>
       <c r="G58" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D59" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E59" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F59">
         <v>0.6</v>
       </c>
       <c r="G59" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E60" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F60">
         <v>0.6</v>
       </c>
       <c r="G60" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D61" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E61" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F61">
         <v>0.6</v>
       </c>
       <c r="G61" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E62" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F62">
         <v>0.66</v>
       </c>
       <c r="G62" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D63" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E63" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F63">
         <v>0.66</v>
       </c>
       <c r="G63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C64" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D64" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E64" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F64">
         <v>0.66</v>
       </c>
       <c r="G64" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D65" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E65" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F65">
         <v>0.66</v>
       </c>
       <c r="G65" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C66" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E66" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F66">
         <v>0.6</v>
       </c>
       <c r="G66" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E67" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F67">
         <v>0.6</v>
       </c>
       <c r="G67" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C68" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D68" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E68" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F68">
         <v>0.6</v>
       </c>
       <c r="G68" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B69" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C69" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D69" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E69" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F69">
         <v>0.6</v>
       </c>
       <c r="G69" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F70">
         <v>0.75</v>
       </c>
       <c r="G70" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D71" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E71" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F71">
         <v>0.75</v>
       </c>
       <c r="G71" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D72" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E72" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F72">
         <v>0.75</v>
       </c>
       <c r="G72" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D73" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E73" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F73">
         <v>0.75</v>
       </c>
       <c r="G73" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C74" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D74" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E74" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F74">
         <v>0.7</v>
       </c>
       <c r="G74" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C75" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D75" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E75" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F75">
         <v>0.7</v>
       </c>
       <c r="G75" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D76" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F76">
         <v>0.7</v>
       </c>
       <c r="G76" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B77" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C77" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D77" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E77" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F77">
         <v>0.7</v>
       </c>
       <c r="G77" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C78" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D78" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E78" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F78">
         <v>0.7</v>
       </c>
       <c r="G78" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C79" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D79" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E79" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F79">
         <v>0.7</v>
       </c>
       <c r="G79" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B80" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C80" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D80" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E80" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F80">
         <v>0.7</v>
       </c>
       <c r="G80" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C81" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D81" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E81" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F81">
         <v>0.7</v>
       </c>
       <c r="G81" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B82" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C82" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D82" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E82" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B83" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C83" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D83" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E83" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B84" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C84" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D84" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E84" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F84">
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B85" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C85" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D85" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E85" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C86" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D86" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E86" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F86">
         <v>0.7</v>
       </c>
       <c r="G86" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C87" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D87" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E87" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F87">
         <v>0.7</v>
       </c>
       <c r="G87" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B88" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C88" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D88" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E88" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F88">
         <v>0.7</v>
       </c>
       <c r="G88" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C89" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D89" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E89" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F89">
         <v>0.7</v>
       </c>
       <c r="G89" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -4057,14 +4020,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4075,224 +4038,224 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
         <v>96</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" t="s">
-        <v>111</v>
-      </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing the infiltration and ventilation idf objects for MMV archetypes
</commit_message>
<xml_diff>
--- a/data/mmv-implementation.xlsx
+++ b/data/mmv-implementation.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamilami\all\buildings\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72A3E5D-2BA1-437F-85F1-E7AF8C776CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4349B629-EB26-408C-AF38-EF54C7E850C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="change" sheetId="1" r:id="rId1"/>
     <sheet name="create" sheetId="5" r:id="rId2"/>
-    <sheet name="AFN" sheetId="8" r:id="rId3"/>
-    <sheet name="EMS program" sheetId="7" r:id="rId4"/>
+    <sheet name="delete" sheetId="9" r:id="rId3"/>
+    <sheet name="AFN" sheetId="8" r:id="rId4"/>
+    <sheet name="EMS program" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="149">
   <si>
     <t>People</t>
   </si>
@@ -477,13 +478,19 @@
   </si>
   <si>
     <t>always_avail</t>
+  </si>
+  <si>
+    <t>ZoneInfiltration:EffectiveLeakageArea</t>
+  </si>
+  <si>
+    <t>ZoneVentilation:DesignFlowRate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,16 +504,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -514,11 +535,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -529,6 +561,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,7 +904,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD63555F-4595-4051-A932-C63C4CE243F7}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
@@ -1939,10 +1973,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B127610-B9C6-4EF6-8F59-487C3311AFAE}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964C1CC5-826A-4834-B9B7-84A48F0779AC}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -4012,7 +4077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15425CF3-EFAC-40C9-A82B-FAFD8DF3F8A1}">
   <dimension ref="A1:C21"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixes to the MMV extension (incl. fixes to #70, see commit description)
The fixes include:
- excluding internal partition surfaces from AFN surfaces (causes error)
- excluding surfaces with boundary type GroundFCfactorMethod from AFN surfaces (causes error)
- excluding zones with no AFN surfaces from MMV zones (infiltration not possible)
- creating as many Sensor_heat and Sensor_cool EMS objects as HVAC zones, getting variable (schedule) directly from the HVAC object (in some cases, each zone could have own thermostat with own schedule)
- creating always_on_MMV and always_off_MMV schedules (typically each idf file has one but their names differ, easier to create own)
- renaming variables like "zone_dict_hvac" to "zone_dict_mmv" to avoid confusion (zone with HVAC system won't necessarily be included in this zone_dict, e.g. if no people object is found)
</commit_message>
<xml_diff>
--- a/data/mmv-implementation.xlsx
+++ b/data/mmv-implementation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamilami\all\buildings\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4349B629-EB26-408C-AF38-EF54C7E850C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFC68E6-7E0A-4004-8209-D194CADA592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="change" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="149">
   <si>
     <t>People</t>
   </si>
@@ -144,27 +144,12 @@
     <t>OutputVariable_or_OutputMeter_Name</t>
   </si>
   <si>
-    <t>Sensor_heat</t>
-  </si>
-  <si>
-    <t>Sensor_cool</t>
-  </si>
-  <si>
-    <t>heating_sch</t>
-  </si>
-  <si>
-    <t>cooling_sch</t>
-  </si>
-  <si>
     <t>Schedule Value</t>
   </si>
   <si>
     <t>Fanger</t>
   </si>
   <si>
-    <t>always_off</t>
-  </si>
-  <si>
     <t>Air_Velocity_Schedule_Name</t>
   </si>
   <si>
@@ -216,36 +201,9 @@
     <t>Wind_Pressure_Coefficient_Curve_Name</t>
   </si>
   <si>
-    <t>HVAC_Sch_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
-    <t>NV_Sch_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
-    <t>Sensor_in_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
-    <t>Sensor_comf_Fan_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
-    <t>Control_HVAC_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
-    <t>Control_NV_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
-    <t>Calculate_openings_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
-    <t>DefineOpening_&lt;hvac zone no.&gt;</t>
-  </si>
-  <si>
     <t>&lt;window name&gt;</t>
   </si>
   <si>
-    <t>&lt;hvac zone name&gt;</t>
-  </si>
-  <si>
     <t>&lt;people object name&gt;</t>
   </si>
   <si>
@@ -330,9 +288,6 @@
     <t>SET Control_&lt;windows&gt; = 0</t>
   </si>
   <si>
-    <t>IF (Sensor_in_X &lt; Sensor_heat)</t>
-  </si>
-  <si>
     <t>DefineOpening_X</t>
   </si>
   <si>
@@ -342,9 +297,6 @@
     <t>SET Control_NV_X = 0</t>
   </si>
   <si>
-    <t>ELSEIF (Sensor_in_X &lt; Sensor_cool)</t>
-  </si>
-  <si>
     <t>SET Control_HVAC_X = 0</t>
   </si>
   <si>
@@ -474,16 +426,64 @@
     <t>surface group</t>
   </si>
   <si>
-    <t>&lt;non-hvac zone name&gt;</t>
-  </si>
-  <si>
-    <t>always_avail</t>
-  </si>
-  <si>
     <t>ZoneInfiltration:EffectiveLeakageArea</t>
   </si>
   <si>
     <t>ZoneVentilation:DesignFlowRate</t>
+  </si>
+  <si>
+    <t>always_on_MMV</t>
+  </si>
+  <si>
+    <t>always_off_MMV</t>
+  </si>
+  <si>
+    <t>&lt;cooling schedule in zone&gt;</t>
+  </si>
+  <si>
+    <t>&lt;heating schedule in zone&gt;</t>
+  </si>
+  <si>
+    <t>IF (Sensor_in_X &lt; Sensor_heat_X)</t>
+  </si>
+  <si>
+    <t>ELSEIF (Sensor_in_X &lt; Sensor_cool_X)</t>
+  </si>
+  <si>
+    <t>&lt;mmv zone name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;non-mmv zone name&gt;</t>
+  </si>
+  <si>
+    <t>HVAC_Sch_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>NV_Sch_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Sensor_heat_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Sensor_cool_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Sensor_in_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Sensor_comf_Fan_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Control_HVAC_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Control_NV_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Calculate_openings_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>DefineOpening_&lt;mmv zone no.&gt;</t>
   </si>
 </sst>
 </file>
@@ -598,8 +598,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FCC55F2-F857-4667-892F-4B3710709F9F}" name="Table2" displayName="Table2" ref="A1:D67" totalsRowShown="0">
-  <autoFilter ref="A1:D67" xr:uid="{E95F4E3E-AEC5-439A-A7A0-FD25B51BF8E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FCC55F2-F857-4667-892F-4B3710709F9F}" name="Table2" displayName="Table2" ref="A1:D73" totalsRowShown="0">
+  <autoFilter ref="A1:D73" xr:uid="{E95F4E3E-AEC5-439A-A7A0-FD25B51BF8E6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8865D9DB-D431-4975-9229-8C6286E87421}" name="object number"/>
     <tableColumn id="2" xr3:uid="{3D54CA2E-DEDC-44BD-903C-115EE860BDB9}" name="idfobject"/>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -951,10 +951,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -965,10 +965,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -979,10 +979,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -996,7 +996,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1010,16 +1010,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD63555F-4595-4051-A932-C63C4CE243F7}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -1105,7 +1105,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1133,7 +1133,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1147,7 +1147,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1175,7 +1175,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1189,7 +1189,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1231,7 +1231,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1315,7 +1315,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1329,7 +1329,7 @@
         <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1343,7 +1343,7 @@
         <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1357,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1371,7 +1371,7 @@
         <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1385,7 +1385,7 @@
         <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1413,7 +1413,7 @@
         <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1441,7 +1441,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1455,7 +1455,7 @@
         <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1469,7 +1469,7 @@
         <v>34</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1477,13 +1477,13 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>63</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1491,13 +1491,13 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1505,10 +1505,10 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>23</v>
@@ -1519,13 +1519,13 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1533,13 +1533,13 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1547,13 +1547,13 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1561,10 +1561,10 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>23</v>
@@ -1575,13 +1575,13 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1589,13 +1589,13 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1603,13 +1603,13 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1617,13 +1617,13 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1631,13 +1631,13 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1645,13 +1645,13 @@
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>65</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1659,13 +1659,13 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1673,13 +1673,13 @@
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1687,13 +1687,13 @@
         <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1701,13 +1701,13 @@
         <v>15</v>
       </c>
       <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C49" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1715,13 +1715,13 @@
         <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1729,13 +1729,13 @@
         <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1743,10 +1743,10 @@
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D52" s="1">
         <v>2</v>
@@ -1757,10 +1757,10 @@
         <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -1771,10 +1771,10 @@
         <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D54" s="1">
         <v>0.6</v>
@@ -1785,10 +1785,10 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -1799,10 +1799,10 @@
         <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -1813,10 +1813,10 @@
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -1827,10 +1827,10 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
@@ -1841,10 +1841,10 @@
         <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D59" s="1">
         <v>0.6</v>
@@ -1855,10 +1855,10 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C60" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
@@ -1869,10 +1869,10 @@
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
@@ -1883,10 +1883,10 @@
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
@@ -1897,13 +1897,13 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1911,13 +1911,13 @@
         <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1925,13 +1925,13 @@
         <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C65" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1939,7 +1939,7 @@
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
         <v>20</v>
@@ -1953,13 +1953,97 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C67" t="s">
         <v>22</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>19</v>
+      </c>
+      <c r="B68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>19</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>19</v>
+      </c>
+      <c r="B70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1976,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B127610-B9C6-4EF6-8F59-487C3311AFAE}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1989,12 +2073,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2022,16 +2106,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2040,2031 +2124,2031 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F2">
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F3">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F4">
         <v>1E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F6">
         <v>1.4E-3</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E7" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F7">
         <v>1.5999999999999999E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F8">
         <v>1.8E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E9" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F9">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G9" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F10">
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="G10" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F11">
         <v>9.6999999999999994E-4</v>
       </c>
       <c r="G11" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F12">
         <v>1.8E-3</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F13">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G13" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F14">
         <v>0.02</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F15">
         <v>0.02</v>
       </c>
       <c r="G15" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F16">
         <v>0.02</v>
       </c>
       <c r="G16" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F17">
         <v>0.02</v>
       </c>
       <c r="G17" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F18">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F19">
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F20">
         <v>0.01</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F21">
         <v>0.04</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" t="s">
         <v>124</v>
-      </c>
-      <c r="B22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" t="s">
-        <v>142</v>
-      </c>
-      <c r="E22" t="s">
-        <v>140</v>
       </c>
       <c r="F22">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" t="s">
         <v>124</v>
-      </c>
-      <c r="B23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" t="s">
-        <v>140</v>
       </c>
       <c r="F23">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" t="s">
         <v>124</v>
-      </c>
-      <c r="B24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" t="s">
-        <v>142</v>
-      </c>
-      <c r="E24" t="s">
-        <v>140</v>
       </c>
       <c r="F24">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" t="s">
         <v>124</v>
-      </c>
-      <c r="B25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" t="s">
-        <v>140</v>
       </c>
       <c r="F25">
         <v>0.02</v>
       </c>
       <c r="G25" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F26">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G26" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F27">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F28">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G28" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F29">
         <v>1.9E-2</v>
       </c>
       <c r="G29" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F30">
         <v>1E-4</v>
       </c>
       <c r="G30" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F31">
         <v>1.5000000000000001E-4</v>
       </c>
       <c r="G31" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F32">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G32" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E33" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F33">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="G33" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F34">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="G34" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F35">
         <v>1.4499999999999999E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D36" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F36">
         <v>2E-3</v>
       </c>
       <c r="G36" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F37">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G37" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F38">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="G38" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F39">
         <v>8.5000000000000006E-4</v>
       </c>
       <c r="G39" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F40">
         <v>1E-3</v>
       </c>
       <c r="G40" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F41">
         <v>2E-3</v>
       </c>
       <c r="G41" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F42">
         <v>1E-4</v>
       </c>
       <c r="G42" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D43" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E43" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F43">
         <v>1.25E-4</v>
       </c>
       <c r="G43" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E44" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F44">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="G44" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E45" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F45">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G45" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E46" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F46">
         <v>0.65</v>
       </c>
       <c r="G46" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E47" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F47">
         <v>0.625</v>
       </c>
       <c r="G47" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E48" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F48">
         <v>0.6</v>
       </c>
       <c r="G48" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E49" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F49">
         <v>0.6</v>
       </c>
       <c r="G49" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E50" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F50">
         <v>0.65</v>
       </c>
       <c r="G50" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E51" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F51">
         <v>0.625</v>
       </c>
       <c r="G51" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E52" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F52">
         <v>0.6</v>
       </c>
       <c r="G52" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D53" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E53" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F53">
         <v>0.6</v>
       </c>
       <c r="G53" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D54" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E54" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F54">
         <v>0.65</v>
       </c>
       <c r="G54" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D55" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E55" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F55">
         <v>0.65500000000000003</v>
       </c>
       <c r="G55" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E56" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F56">
         <v>0.66</v>
       </c>
       <c r="G56" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E57" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F57">
         <v>0.66</v>
       </c>
       <c r="G57" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D58" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E58" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F58">
         <v>0.6</v>
       </c>
       <c r="G58" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E59" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F59">
         <v>0.6</v>
       </c>
       <c r="G59" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D60" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E60" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F60">
         <v>0.6</v>
       </c>
       <c r="G60" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E61" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F61">
         <v>0.6</v>
       </c>
       <c r="G61" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C62" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E62" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F62">
         <v>0.66</v>
       </c>
       <c r="G62" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C63" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E63" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F63">
         <v>0.66</v>
       </c>
       <c r="G63" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E64" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F64">
         <v>0.66</v>
       </c>
       <c r="G64" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E65" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F65">
         <v>0.66</v>
       </c>
       <c r="G65" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E66" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F66">
         <v>0.6</v>
       </c>
       <c r="G66" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E67" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F67">
         <v>0.6</v>
       </c>
       <c r="G67" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C68" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D68" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E68" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F68">
         <v>0.6</v>
       </c>
       <c r="G68" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C69" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D69" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E69" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F69">
         <v>0.6</v>
       </c>
       <c r="G69" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D70" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E70" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F70">
         <v>0.75</v>
       </c>
       <c r="G70" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C71" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D71" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E71" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F71">
         <v>0.75</v>
       </c>
       <c r="G71" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C72" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D72" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E72" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F72">
         <v>0.75</v>
       </c>
       <c r="G72" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D73" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E73" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F73">
         <v>0.75</v>
       </c>
       <c r="G73" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>111</v>
+      </c>
+      <c r="B74" t="s">
+        <v>94</v>
+      </c>
+      <c r="C74" t="s">
+        <v>98</v>
+      </c>
+      <c r="D74" t="s">
         <v>127</v>
       </c>
-      <c r="B74" t="s">
-        <v>110</v>
-      </c>
-      <c r="C74" t="s">
-        <v>114</v>
-      </c>
-      <c r="D74" t="s">
-        <v>143</v>
-      </c>
       <c r="E74" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F74">
         <v>0.7</v>
       </c>
       <c r="G74" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" t="s">
+        <v>95</v>
+      </c>
+      <c r="C75" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" t="s">
         <v>127</v>
       </c>
-      <c r="B75" t="s">
-        <v>111</v>
-      </c>
-      <c r="C75" t="s">
-        <v>115</v>
-      </c>
-      <c r="D75" t="s">
-        <v>143</v>
-      </c>
       <c r="E75" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F75">
         <v>0.7</v>
       </c>
       <c r="G75" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" t="s">
+        <v>100</v>
+      </c>
+      <c r="D76" t="s">
         <v>127</v>
       </c>
-      <c r="B76" t="s">
-        <v>112</v>
-      </c>
-      <c r="C76" t="s">
-        <v>116</v>
-      </c>
-      <c r="D76" t="s">
-        <v>143</v>
-      </c>
       <c r="E76" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F76">
         <v>0.7</v>
       </c>
       <c r="G76" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" t="s">
+        <v>101</v>
+      </c>
+      <c r="D77" t="s">
         <v>127</v>
       </c>
-      <c r="B77" t="s">
-        <v>113</v>
-      </c>
-      <c r="C77" t="s">
-        <v>117</v>
-      </c>
-      <c r="D77" t="s">
-        <v>143</v>
-      </c>
       <c r="E77" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F77">
         <v>0.7</v>
       </c>
       <c r="G77" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D78" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E78" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F78">
         <v>0.7</v>
       </c>
       <c r="G78" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C79" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D79" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E79" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F79">
         <v>0.7</v>
       </c>
       <c r="G79" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B80" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C80" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D80" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E80" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F80">
         <v>0.7</v>
       </c>
       <c r="G80" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C81" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D81" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E81" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F81">
         <v>0.7</v>
       </c>
       <c r="G81" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B82" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D82" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E82" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B83" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D83" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E83" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B84" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D84" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E84" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F84">
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E85" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B86" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C86" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D86" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E86" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F86">
         <v>0.7</v>
       </c>
       <c r="G86" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C87" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D87" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E87" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F87">
         <v>0.7</v>
       </c>
       <c r="G87" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B88" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C88" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D88" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E88" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F88">
         <v>0.7</v>
       </c>
       <c r="G88" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B89" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D89" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E89" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F89">
         <v>0.7</v>
       </c>
       <c r="G89" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4082,14 +4166,14 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -4105,222 +4189,222 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
         <v>92</v>
       </c>
-      <c r="B6" t="s">
-        <v>108</v>
-      </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="B7" t="s">
-        <v>108</v>
-      </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
         <v>92</v>
       </c>
-      <c r="B8" t="s">
-        <v>108</v>
-      </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" t="s">
-        <v>108</v>
-      </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" t="s">
-        <v>108</v>
-      </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
         <v>92</v>
       </c>
-      <c r="B11" t="s">
-        <v>108</v>
-      </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
         <v>92</v>
       </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
         <v>92</v>
       </c>
-      <c r="B13" t="s">
-        <v>108</v>
-      </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
         <v>92</v>
       </c>
-      <c r="B14" t="s">
-        <v>108</v>
-      </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
         <v>92</v>
       </c>
-      <c r="B15" t="s">
-        <v>108</v>
-      </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
         <v>92</v>
       </c>
-      <c r="B16" t="s">
-        <v>108</v>
-      </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
         <v>92</v>
       </c>
-      <c r="B17" t="s">
-        <v>108</v>
-      </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
         <v>92</v>
       </c>
-      <c r="B18" t="s">
-        <v>108</v>
-      </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
         <v>92</v>
       </c>
-      <c r="B19" t="s">
-        <v>108</v>
-      </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
         <v>92</v>
       </c>
-      <c r="B20" t="s">
-        <v>108</v>
-      </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
         <v>92</v>
       </c>
-      <c r="B21" t="s">
-        <v>108</v>
-      </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the code to fix issue #78 and simplify the MMV procedure
</commit_message>
<xml_diff>
--- a/data/mmv-implementation.xlsx
+++ b/data/mmv-implementation.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamilami\all\buildings\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFC68E6-7E0A-4004-8209-D194CADA592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8FC85F-DE35-42EA-9DF6-F28042D560F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="change" sheetId="1" r:id="rId1"/>
-    <sheet name="create" sheetId="5" r:id="rId2"/>
-    <sheet name="delete" sheetId="9" r:id="rId3"/>
-    <sheet name="AFN" sheetId="8" r:id="rId4"/>
-    <sheet name="EMS program" sheetId="7" r:id="rId5"/>
+    <sheet name="delete" sheetId="9" r:id="rId2"/>
+    <sheet name="create-AFN" sheetId="5" r:id="rId3"/>
+    <sheet name="create-MMV" sheetId="11" r:id="rId4"/>
+    <sheet name="AFN" sheetId="8" r:id="rId5"/>
+    <sheet name="EMS program" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="147">
   <si>
     <t>People</t>
   </si>
@@ -177,12 +178,6 @@
     <t>Actuated_Component_Control_Type</t>
   </si>
   <si>
-    <t>AirFlow Network Window/Door Opening</t>
-  </si>
-  <si>
-    <t>Venting Opening Factor</t>
-  </si>
-  <si>
     <t>EnergyManagementSystem:ProgramCallingManager</t>
   </si>
   <si>
@@ -201,9 +196,6 @@
     <t>Wind_Pressure_Coefficient_Curve_Name</t>
   </si>
   <si>
-    <t>&lt;window name&gt;</t>
-  </si>
-  <si>
     <t>&lt;people object name&gt;</t>
   </si>
   <si>
@@ -285,9 +277,6 @@
     <t>Program_Line_2</t>
   </si>
   <si>
-    <t>SET Control_&lt;windows&gt; = 0</t>
-  </si>
-  <si>
     <t>DefineOpening_X</t>
   </si>
   <si>
@@ -306,9 +295,6 @@
     <t>IF (Sensor_in_X &gt; Sensor_out) &amp;&amp; (Sensor_comf_Fan_X &lt; 20)</t>
   </si>
   <si>
-    <t>SET Control_&lt;windows&gt; = 0.27</t>
-  </si>
-  <si>
     <t>ENDIF</t>
   </si>
   <si>
@@ -318,9 +304,6 @@
     <t>Program_Line_&lt;next&gt;</t>
   </si>
   <si>
-    <t>Control_Win_&lt;window no.&gt;</t>
-  </si>
-  <si>
     <t>ZEB</t>
   </si>
   <si>
@@ -432,12 +415,6 @@
     <t>ZoneVentilation:DesignFlowRate</t>
   </si>
   <si>
-    <t>always_on_MMV</t>
-  </si>
-  <si>
-    <t>always_off_MMV</t>
-  </si>
-  <si>
     <t>&lt;cooling schedule in zone&gt;</t>
   </si>
   <si>
@@ -484,6 +461,24 @@
   </si>
   <si>
     <t>DefineOpening_&lt;mmv zone no.&gt;</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>WindowDoor_Opening_Factor_or_Crack_Factor</t>
+  </si>
+  <si>
+    <t>&lt;opening factor&gt;</t>
+  </si>
+  <si>
+    <t>ZoneInfiltration:DesignFlowRate</t>
+  </si>
+  <si>
+    <t>always_off_BuildME</t>
+  </si>
+  <si>
+    <t>always_on_BuildME</t>
   </si>
 </sst>
 </file>
@@ -567,7 +562,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -598,19 +596,34 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FCC55F2-F857-4667-892F-4B3710709F9F}" name="Table2" displayName="Table2" ref="A1:D73" totalsRowShown="0">
-  <autoFilter ref="A1:D73" xr:uid="{E95F4E3E-AEC5-439A-A7A0-FD25B51BF8E6}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FCC55F2-F857-4667-892F-4B3710709F9F}" name="Table2" displayName="Table2" ref="A1:E44" totalsRowShown="0">
+  <autoFilter ref="A1:E44" xr:uid="{E95F4E3E-AEC5-439A-A7A0-FD25B51BF8E6}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8865D9DB-D431-4975-9229-8C6286E87421}" name="object number"/>
     <tableColumn id="2" xr3:uid="{3D54CA2E-DEDC-44BD-903C-115EE860BDB9}" name="idfobject"/>
     <tableColumn id="3" xr3:uid="{358EA3EF-7D28-4C28-B118-B55C77676487}" name="objectfield"/>
-    <tableColumn id="4" xr3:uid="{FE8E3E02-0CF3-46F0-B145-E3CB7E4D4767}" name="value" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{FE8E3E02-0CF3-46F0-B145-E3CB7E4D4767}" name="value" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{7645A35D-3D40-4BD0-A6F9-112B2855C530}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BE1097E5-A91C-4D73-9CE2-71B2147FB343}" name="Table27" displayName="Table27" ref="A1:E27" totalsRowShown="0">
+  <autoFilter ref="A1:E27" xr:uid="{BE1097E5-A91C-4D73-9CE2-71B2147FB343}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4F12D81B-EEA0-412D-9230-BCF6117A2500}" name="object number"/>
+    <tableColumn id="2" xr3:uid="{7E026F3A-2D9A-4CB0-BF64-932786FB1063}" name="idfobject"/>
+    <tableColumn id="3" xr3:uid="{466FC7A3-A271-4EF2-91AE-EB857FE0B22D}" name="objectfield"/>
+    <tableColumn id="4" xr3:uid="{AF204025-890B-4757-A788-55D7E538D345}" name="value" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{487922BA-75E6-451A-BC0D-D2F2C79D2199}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF6D813E-4C14-47A0-803D-8C4A345B6D7F}" name="Table1" displayName="Table1" ref="A1:G89" totalsRowShown="0">
   <autoFilter ref="A1:G89" xr:uid="{194E0B9C-D9C4-483A-AF51-AB14A5D2C1C8}"/>
   <tableColumns count="7">
@@ -626,9 +639,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14574C82-F844-4968-A166-39954FB3AAE8}" name="Table3" displayName="Table3" ref="A1:C21" totalsRowShown="0">
-  <autoFilter ref="A1:C21" xr:uid="{8918CADC-2BBA-4F5E-8B01-D240A08E350A}"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14574C82-F844-4968-A166-39954FB3AAE8}" name="Table3" displayName="Table3" ref="A1:C17" totalsRowShown="0">
+  <autoFilter ref="A1:C17" xr:uid="{8918CADC-2BBA-4F5E-8B01-D240A08E350A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D77B4FE5-A5E4-4F19-AAC9-7726347B3C01}" name="idfobject"/>
     <tableColumn id="2" xr3:uid="{606412C4-D27E-4F4C-B846-57A7ECD0AEF3}" name="objectfield"/>
@@ -903,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,7 +967,7 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -968,7 +981,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -996,7 +1009,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1009,22 +1022,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B127610-B9C6-4EF6-8F59-487C3311AFAE}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD63555F-4595-4051-A932-C63C4CE243F7}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" customWidth="1"/>
     <col min="2" max="2" width="50.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1037,8 +1086,11 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1052,7 +1104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1066,7 +1118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1080,7 +1132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1094,7 +1146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1105,10 +1157,10 @@
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -1122,7 +1174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -1132,11 +1184,11 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -1147,10 +1199,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -1164,7 +1216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -1175,10 +1227,10 @@
         <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1189,10 +1241,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1206,7 +1258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1220,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1231,10 +1283,10 @@
         <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1267,13 +1319,13 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
+      <c r="D18" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1281,69 +1333,69 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>141</v>
+      <c r="D21" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>134</v>
+        <v>62</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>35</v>
+        <v>63</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1351,13 +1403,13 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>142</v>
+        <v>64</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.6</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1365,13 +1417,13 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>133</v>
+        <v>65</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1379,670 +1431,264 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>143</v>
+        <v>72</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>137</v>
+        <v>67</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>144</v>
+        <v>69</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>139</v>
+        <v>57</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>35</v>
+        <v>142</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>93</v>
+        <v>26</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>54</v>
+        <v>10</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>14</v>
-      </c>
-      <c r="B46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>15</v>
-      </c>
-      <c r="B48" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>15</v>
-      </c>
-      <c r="B49" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>16</v>
-      </c>
-      <c r="B50" t="s">
-        <v>63</v>
-      </c>
-      <c r="C50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>17</v>
-      </c>
-      <c r="B51" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>17</v>
-      </c>
-      <c r="B52" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" t="s">
-        <v>65</v>
-      </c>
-      <c r="D52" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>17</v>
-      </c>
-      <c r="B53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>17</v>
-      </c>
-      <c r="B54" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>17</v>
-      </c>
-      <c r="B55" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>17</v>
-      </c>
-      <c r="B56" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>17</v>
-      </c>
-      <c r="B57" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" t="s">
-        <v>75</v>
-      </c>
-      <c r="D57" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>17</v>
-      </c>
-      <c r="B58" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" t="s">
-        <v>70</v>
-      </c>
-      <c r="D58" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>17</v>
-      </c>
-      <c r="B59" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" t="s">
-        <v>71</v>
-      </c>
-      <c r="D59" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>17</v>
-      </c>
-      <c r="B60" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>17</v>
-      </c>
-      <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" t="s">
-        <v>73</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>17</v>
-      </c>
-      <c r="B62" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" t="s">
-        <v>76</v>
-      </c>
-      <c r="D62" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>18</v>
-      </c>
-      <c r="B63" t="s">
-        <v>58</v>
-      </c>
-      <c r="C63" t="s">
-        <v>59</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>18</v>
-      </c>
-      <c r="B64" t="s">
-        <v>58</v>
-      </c>
-      <c r="C64" t="s">
-        <v>60</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>18</v>
-      </c>
-      <c r="B65" t="s">
-        <v>58</v>
-      </c>
-      <c r="C65" t="s">
-        <v>61</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>18</v>
-      </c>
-      <c r="B66" t="s">
-        <v>58</v>
-      </c>
-      <c r="C66" t="s">
-        <v>20</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>18</v>
-      </c>
-      <c r="B67" t="s">
-        <v>58</v>
-      </c>
-      <c r="C67" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>19</v>
-      </c>
-      <c r="B68" t="s">
-        <v>23</v>
-      </c>
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>19</v>
-      </c>
-      <c r="B69" t="s">
-        <v>23</v>
-      </c>
-      <c r="C69" t="s">
-        <v>24</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <v>19</v>
-      </c>
-      <c r="B70" t="s">
-        <v>23</v>
-      </c>
-      <c r="C70" t="s">
         <v>26</v>
       </c>
-      <c r="D70" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>20</v>
-      </c>
-      <c r="B71" t="s">
-        <v>23</v>
-      </c>
-      <c r="C71" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>20</v>
-      </c>
-      <c r="B72" t="s">
-        <v>23</v>
-      </c>
-      <c r="C72" t="s">
-        <v>24</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>20</v>
-      </c>
-      <c r="B73" t="s">
-        <v>23</v>
-      </c>
-      <c r="C73" t="s">
-        <v>26</v>
-      </c>
-      <c r="D73" s="1">
+      <c r="D44" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2056,38 +1702,416 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B127610-B9C6-4EF6-8F59-487C3311AFAE}">
-  <dimension ref="A1:A3"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F6FFD7-421E-46D7-80CE-7FB68807673A}">
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B25" sqref="B25:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>130</v>
-      </c>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964C1CC5-826A-4834-B9B7-84A48F0779AC}">
   <dimension ref="A1:G89"/>
   <sheetViews>
@@ -2106,16 +2130,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2124,2031 +2148,2031 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F2">
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F3">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F4">
         <v>1E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F6">
         <v>1.4E-3</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F7">
         <v>1.5999999999999999E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F8">
         <v>1.8E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F9">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F10">
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="G10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F11">
         <v>9.6999999999999994E-4</v>
       </c>
       <c r="G11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F12">
         <v>1.8E-3</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F13">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F14">
         <v>0.02</v>
       </c>
       <c r="G14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F15">
         <v>0.02</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E16" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F16">
         <v>0.02</v>
       </c>
       <c r="G16" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F17">
         <v>0.02</v>
       </c>
       <c r="G17" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F18">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F19">
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F20">
         <v>0.01</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F21">
         <v>0.04</v>
       </c>
       <c r="G21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F22">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="G22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F23">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G23" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F24">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F25">
         <v>0.02</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E26" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F26">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G26" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F27">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G27" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F28">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G28" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F29">
         <v>1.9E-2</v>
       </c>
       <c r="G29" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E30" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F30">
         <v>1E-4</v>
       </c>
       <c r="G30" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D31" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E31" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F31">
         <v>1.5000000000000001E-4</v>
       </c>
       <c r="G31" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F32">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G32" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F33">
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="G33" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D34" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F34">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="G34" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F35">
         <v>1.4499999999999999E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D36" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F36">
         <v>2E-3</v>
       </c>
       <c r="G36" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F37">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G37" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E38" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F38">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="G38" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E39" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F39">
         <v>8.5000000000000006E-4</v>
       </c>
       <c r="G39" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F40">
         <v>1E-3</v>
       </c>
       <c r="G40" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D41" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E41" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F41">
         <v>2E-3</v>
       </c>
       <c r="G41" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D42" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E42" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F42">
         <v>1E-4</v>
       </c>
       <c r="G42" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E43" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F43">
         <v>1.25E-4</v>
       </c>
       <c r="G43" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F44">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="G44" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D45" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F45">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G45" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E46" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F46">
         <v>0.65</v>
       </c>
       <c r="G46" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E47" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F47">
         <v>0.625</v>
       </c>
       <c r="G47" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D48" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E48" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F48">
         <v>0.6</v>
       </c>
       <c r="G48" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D49" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E49" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F49">
         <v>0.6</v>
       </c>
       <c r="G49" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E50" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F50">
         <v>0.65</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D51" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F51">
         <v>0.625</v>
       </c>
       <c r="G51" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E52" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F52">
         <v>0.6</v>
       </c>
       <c r="G52" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D53" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E53" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F53">
         <v>0.6</v>
       </c>
       <c r="G53" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C54" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D54" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E54" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F54">
         <v>0.65</v>
       </c>
       <c r="G54" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D55" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E55" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F55">
         <v>0.65500000000000003</v>
       </c>
       <c r="G55" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C56" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D56" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E56" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F56">
         <v>0.66</v>
       </c>
       <c r="G56" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D57" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E57" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F57">
         <v>0.66</v>
       </c>
       <c r="G57" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D58" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E58" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F58">
         <v>0.6</v>
       </c>
       <c r="G58" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D59" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E59" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F59">
         <v>0.6</v>
       </c>
       <c r="G59" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C60" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E60" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F60">
         <v>0.6</v>
       </c>
       <c r="G60" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D61" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E61" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F61">
         <v>0.6</v>
       </c>
       <c r="G61" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D62" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E62" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F62">
         <v>0.66</v>
       </c>
       <c r="G62" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D63" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E63" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F63">
         <v>0.66</v>
       </c>
       <c r="G63" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C64" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D64" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E64" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F64">
         <v>0.66</v>
       </c>
       <c r="G64" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B65" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D65" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E65" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F65">
         <v>0.66</v>
       </c>
       <c r="G65" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D66" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E66" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F66">
         <v>0.6</v>
       </c>
       <c r="G66" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D67" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E67" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F67">
         <v>0.6</v>
       </c>
       <c r="G67" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D68" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E68" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F68">
         <v>0.6</v>
       </c>
       <c r="G68" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B69" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D69" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E69" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F69">
         <v>0.6</v>
       </c>
       <c r="G69" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C70" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D70" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E70" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F70">
         <v>0.75</v>
       </c>
       <c r="G70" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B71" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D71" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E71" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F71">
         <v>0.75</v>
       </c>
       <c r="G71" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B72" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D72" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E72" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F72">
         <v>0.75</v>
       </c>
       <c r="G72" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C73" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D73" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E73" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F73">
         <v>0.75</v>
       </c>
       <c r="G73" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C74" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D74" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E74" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F74">
         <v>0.7</v>
       </c>
       <c r="G74" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C75" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D75" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E75" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F75">
         <v>0.7</v>
       </c>
       <c r="G75" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C76" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D76" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E76" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F76">
         <v>0.7</v>
       </c>
       <c r="G76" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C77" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D77" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E77" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F77">
         <v>0.7</v>
       </c>
       <c r="G77" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C78" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D78" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E78" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F78">
         <v>0.7</v>
       </c>
       <c r="G78" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D79" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E79" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F79">
         <v>0.7</v>
       </c>
       <c r="G79" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C80" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D80" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E80" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F80">
         <v>0.7</v>
       </c>
       <c r="G80" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D81" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E81" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F81">
         <v>0.7</v>
       </c>
       <c r="G81" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C82" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D82" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E82" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C83" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D83" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E83" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C84" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D84" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E84" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F84">
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C85" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D85" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E85" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
       <c r="G85" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D86" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E86" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F86">
         <v>0.7</v>
       </c>
       <c r="G86" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C87" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D87" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E87" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F87">
         <v>0.7</v>
       </c>
       <c r="G87" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B88" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C88" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D88" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E88" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F88">
         <v>0.7</v>
       </c>
       <c r="G88" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D89" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E89" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F89">
         <v>0.7</v>
       </c>
       <c r="G89" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4161,9 +4185,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15425CF3-EFAC-40C9-A82B-FAFD8DF3F8A1}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -4189,222 +4213,178 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>